<commit_message>
intermediate commit with work on Dutch language SIAM for RAP3
</commit_message>
<xml_diff>
--- a/RAP3/SIAMpop.xlsx
+++ b/RAP3/SIAMpop.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Organization</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>Middlepart</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Student</t>
   </si>
 </sst>
 </file>
@@ -587,7 +593,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +650,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="str">
-        <f t="shared" ref="A3:A5" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
+        <f t="shared" ref="A3" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
         <v>Stef Joosten</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -668,7 +674,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="str">
-        <f t="shared" ref="A5" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
+        <f t="shared" ref="A5:A7" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van der Wetering</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -683,13 +689,19 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="str">
-        <f>IF($B6="","",CONCATENATE($B6," ",$C6))</f>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>Jan Student</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="str">
-        <f>IF($B7="","",CONCATENATE($B7," ",$C7))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -913,18 +925,18 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Acc_Jan</v>
       </c>
       <c r="B17" s="5" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Jan Student</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D17" s="7" t="str">
         <f>$A6</f>
-        <v/>
+        <v>Jan Student</v>
       </c>
       <c r="E17" s="7" t="str">
         <f t="shared" si="5"/>

</xml_diff>

<commit_message>
RAP3 - update w.r.t. SIAM integration
</commit_message>
<xml_diff>
--- a/RAP3/SIAMpop.xlsx
+++ b/RAP3/SIAMpop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="11655" windowHeight="5400"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="11652" windowHeight="5400"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
@@ -13,41 +13,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Auteur</author>
-  </authors>
-  <commentList>
-    <comment ref="J12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Rieks: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>There should be at most 1 autoLoginAccount</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Organization</t>
   </si>
@@ -76,9 +43,6 @@
     <t>Role</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>personFirstName</t>
   </si>
   <si>
@@ -91,12 +55,6 @@
     <t>personLastName</t>
   </si>
   <si>
-    <t>ExcelImporter</t>
-  </si>
-  <si>
-    <t>ExecEngineer</t>
-  </si>
-  <si>
     <t>[OrganizationReg]</t>
   </si>
   <si>
@@ -136,9 +94,6 @@
     <t>welkom</t>
   </si>
   <si>
-    <t>SystemAdmin</t>
-  </si>
-  <si>
     <t>Lloyd</t>
   </si>
   <si>
@@ -170,13 +125,22 @@
   </si>
   <si>
     <t>Student</t>
+  </si>
+  <si>
+    <t>Account manager</t>
+  </si>
+  <si>
+    <t>Tutor</t>
+  </si>
+  <si>
+    <t>de</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,19 +154,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -258,9 +209,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -277,21 +228,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
-    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -304,9 +252,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -344,7 +292,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -416,7 +364,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -589,131 +537,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="3" customWidth="1"/>
-    <col min="7" max="9" width="13.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="str">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="str">
         <f t="shared" ref="A3" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
         <v>Stef Joosten</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="str">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="str">
         <f>IF($B4="","",CONCATENATE($B4," ",IF($C4="",D4,CONCATENATE($C4," ",$D4))))</f>
         <v>Lloyd Rutledge</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="str">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="str">
         <f t="shared" ref="A5:A7" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van der Wetering</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Jan de Student</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>Jan Student</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="str">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -721,17 +670,16 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -739,30 +687,29 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="str">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>OUNL</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="str">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="str">
         <f>IF($B11="","",$B11)</f>
         <v/>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -773,32 +720,25 @@
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="6" t="str">
-        <f>IF((ROWS($J$14:$J$17)-COUNTBLANK($J$14:$J$17))=0,"","autoLoginAccount")</f>
-        <v/>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -824,18 +764,11 @@
         <v>8</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J13" s="2" t="str">
-        <f>$A13</f>
-        <v>Account</v>
-      </c>
-      <c r="K13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="str">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="str">
         <f>IF($B14="","",CONCATENATE("Acc_",$B3))</f>
         <v>Acc_Stef</v>
       </c>
@@ -844,36 +777,26 @@
         <v>Stef Joosten</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="7" t="str">
+        <v>25</v>
+      </c>
+      <c r="D14" s="6" t="str">
         <f>$A3</f>
         <v>Stef Joosten</v>
       </c>
-      <c r="E14" s="7" t="str">
+      <c r="E14" s="6" t="str">
         <f>$A$10</f>
         <v>OUNL</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="7"/>
-      <c r="K14" t="str">
+        <v>38</v>
+      </c>
+      <c r="I14" s="3" t="str">
         <f>$A14</f>
         <v>Acc_Stef</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="str">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="str">
         <f t="shared" ref="A15:A17" si="2">IF($B15="","",CONCATENATE("Acc_",$B4))</f>
         <v>Acc_Lloyd</v>
       </c>
@@ -882,23 +805,25 @@
         <v>Lloyd Rutledge</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="7" t="str">
+        <v>25</v>
+      </c>
+      <c r="D15" s="6" t="str">
         <f t="shared" ref="D15" si="4">$A4</f>
         <v>Lloyd Rutledge</v>
       </c>
-      <c r="E15" s="7" t="str">
+      <c r="E15" s="6" t="str">
         <f t="shared" ref="E15:E18" si="5">$A$10</f>
         <v>OUNL</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="G15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="str">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Rogier</v>
       </c>
@@ -907,64 +832,59 @@
         <v>Rogier van der Wetering</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="7" t="str">
+        <v>25</v>
+      </c>
+      <c r="D16" s="6" t="str">
         <f t="shared" ref="D16" si="6">$A5</f>
         <v>Rogier van der Wetering</v>
       </c>
-      <c r="E16" s="7" t="str">
+      <c r="E16" s="6" t="str">
         <f t="shared" si="5"/>
         <v>OUNL</v>
       </c>
+      <c r="F16" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="G16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="str">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Jan</v>
       </c>
       <c r="B17" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>Jan Student</v>
+        <v>Jan de Student</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="7" t="str">
+        <v>25</v>
+      </c>
+      <c r="D17" s="6" t="str">
         <f>$A6</f>
-        <v>Jan Student</v>
-      </c>
-      <c r="E17" s="7" t="str">
+        <v>Jan de Student</v>
+      </c>
+      <c r="E17" s="6" t="str">
         <f t="shared" si="5"/>
         <v>OUNL</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="str">
-        <f>IF($B18="","",CONCATENATE("Acc_",$B18))</f>
-        <v/>
-      </c>
-      <c r="D18" s="7" t="str">
-        <f>$A7</f>
-        <v/>
-      </c>
-      <c r="E18" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>OUNL</v>
-      </c>
-      <c r="J18" s="7"/>
+      <c r="F17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
assign various roles to accounts
</commit_message>
<xml_diff>
--- a/RAP3/SIAMpop.xlsx
+++ b/RAP3/SIAMpop.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="11655" windowHeight="5400"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="11655" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Organization</t>
   </si>
@@ -163,13 +163,16 @@
     <t>Open Universiteit Nederland</t>
   </si>
   <si>
-    <t>Middlepart</t>
-  </si>
-  <si>
     <t>Jan</t>
   </si>
   <si>
     <t>Student</t>
+  </si>
+  <si>
+    <t>[Role,]</t>
+  </si>
+  <si>
+    <t>User,Tutor</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,9 +638,7 @@
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
@@ -693,10 +694,10 @@
         <v>Jan Student</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -818,7 +819,7 @@
         <v>8</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>8</v>
@@ -858,7 +859,7 @@
         <v>29</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>14</v>
@@ -893,7 +894,10 @@
         <v>OUNL</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>9</v>
+        <v>41</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="J15" s="7"/>
     </row>
@@ -918,7 +922,10 @@
         <v>OUNL</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>9</v>
+        <v>41</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="J16" s="7"/>
     </row>
@@ -944,6 +951,9 @@
       </c>
       <c r="G17" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="J17" s="7"/>
     </row>

</xml_diff>

<commit_message>
make interfaces for creating and maintaining scripts.
</commit_message>
<xml_diff>
--- a/RAP3/SIAMpop.xlsx
+++ b/RAP3/SIAMpop.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="11652" windowHeight="5400"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="11655" windowHeight="5400"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -237,9 +237,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
+    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -252,9 +252,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -292,7 +292,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -364,7 +364,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -541,22 +541,22 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -575,7 +575,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -594,7 +594,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="str">
         <f t="shared" ref="A3" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
         <v>Stef Joosten</v>
@@ -606,7 +606,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="str">
         <f>IF($B4="","",CONCATENATE($B4," ",IF($C4="",D4,CONCATENATE($C4," ",$D4))))</f>
         <v>Lloyd Rutledge</v>
@@ -618,7 +618,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="str">
         <f t="shared" ref="A5:A7" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van der Wetering</v>
@@ -633,7 +633,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Jan de Student</v>
@@ -648,13 +648,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -671,7 +671,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +688,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>OUNL</v>
@@ -701,7 +701,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="str">
         <f>IF($B11="","",$B11)</f>
         <v/>
@@ -709,7 +709,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -738,7 +738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -767,7 +767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f>IF($B14="","",CONCATENATE("Acc_",$B3))</f>
         <v>Acc_Stef</v>
@@ -795,7 +795,7 @@
         <v>Acc_Stef</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="str">
         <f t="shared" ref="A15:A17" si="2">IF($B15="","",CONCATENATE("Acc_",$B4))</f>
         <v>Acc_Lloyd</v>
@@ -812,7 +812,7 @@
         <v>Lloyd Rutledge</v>
       </c>
       <c r="E15" s="6" t="str">
-        <f t="shared" ref="E15:E18" si="5">$A$10</f>
+        <f t="shared" ref="E15:E17" si="5">$A$10</f>
         <v>OUNL</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -822,7 +822,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Rogier</v>
@@ -849,7 +849,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Acc_Jan</v>
@@ -873,7 +873,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>

</xml_diff>

<commit_message>
add crud restrictions to the interfaces in RAP3.
</commit_message>
<xml_diff>
--- a/RAP3/SIAMpop.xlsx
+++ b/RAP3/SIAMpop.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>Organization</t>
   </si>
@@ -541,7 +541,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,9 +763,7 @@
       <c r="H13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
@@ -790,9 +788,8 @@
       <c r="F14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="3" t="str">
-        <f>$A14</f>
-        <v>Acc_Stef</v>
+      <c r="H14" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -817,9 +814,6 @@
       </c>
       <c r="F15" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
upload files and reorganize SIAM by means of `SIAM_importer.adl`
</commit_message>
<xml_diff>
--- a/RAP3/SIAMpop.xlsx
+++ b/RAP3/SIAMpop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="11655" windowHeight="5400"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="11655" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
@@ -127,13 +127,13 @@
     <t>Student</t>
   </si>
   <si>
-    <t>Account manager</t>
-  </si>
-  <si>
     <t>Tutor</t>
   </si>
   <si>
     <t>de</t>
+  </si>
+  <si>
+    <t>AccountMgr</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
         <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>36</v>
@@ -786,7 +786,7 @@
         <v>OUNL</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>36</v>
@@ -813,7 +813,7 @@
         <v>OUNL</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -837,10 +837,10 @@
         <v>OUNL</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
results of XP-session of Michiel and Stef
</commit_message>
<xml_diff>
--- a/RAP3/SIAMpop.xlsx
+++ b/RAP3/SIAMpop.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>Organization</t>
   </si>
@@ -134,6 +134,24 @@
   </si>
   <si>
     <t>AccountMgr</t>
+  </si>
+  <si>
+    <t>Debbie Tarenskeen</t>
+  </si>
+  <si>
+    <t>Debbie</t>
+  </si>
+  <si>
+    <t>Tarenskeen</t>
+  </si>
+  <si>
+    <t>Acc_Debbie</t>
+  </si>
+  <si>
+    <t>HAN</t>
+  </si>
+  <si>
+    <t>Hogeschool Arnhem Nijmegen</t>
   </si>
 </sst>
 </file>
@@ -211,7 +229,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -234,6 +252,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -541,7 +562,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,9 +670,14 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -702,11 +728,15 @@
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="str">
-        <f>IF($B11="","",$B11)</f>
-        <v/>
-      </c>
-      <c r="C11" s="4"/>
+      <c r="A11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
@@ -868,13 +898,30 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="I18"/>
     </row>
   </sheetData>

</xml_diff>